<commit_message>
still need to fix linear regression on modelcode
</commit_message>
<xml_diff>
--- a/Ensemble/ExperimentalModels/model_metrics.xlsx
+++ b/Ensemble/ExperimentalModels/model_metrics.xlsx
@@ -383,13 +383,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:11">
       <c r="B1" s="1">
         <v>1</v>
       </c>
@@ -405,65 +405,125 @@
       <c r="F1" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" s="1">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>30.64728814967599</v>
+        <v>28.98029672317424</v>
       </c>
       <c r="C2">
-        <v>29.84640153843559</v>
+        <v>36.70850919668717</v>
       </c>
       <c r="D2">
-        <v>40.4679834113933</v>
+        <v>37.96986392644682</v>
       </c>
       <c r="E2">
-        <v>45.4101556159583</v>
+        <v>31.22592845419224</v>
       </c>
       <c r="F2">
-        <v>41.22254011010967</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>43.61157316185502</v>
+      </c>
+      <c r="G2">
+        <v>30.27784069838451</v>
+      </c>
+      <c r="H2">
+        <v>31.30217745473083</v>
+      </c>
+      <c r="I2">
+        <v>39.61213871867896</v>
+      </c>
+      <c r="J2">
+        <v>42.51503485461354</v>
+      </c>
+      <c r="K2">
+        <v>54.25680821473518</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.5112947281812048</v>
+        <v>0.5793310029159989</v>
       </c>
       <c r="C3">
-        <v>0.5969839375289978</v>
+        <v>0.6828392768481389</v>
       </c>
       <c r="D3">
-        <v>0.6541700076993781</v>
+        <v>0.7109865587139155</v>
       </c>
       <c r="E3">
-        <v>0.6482268967453213</v>
+        <v>0.5587914946739748</v>
       </c>
       <c r="F3">
-        <v>0.6627381003334535</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>0.5625940117129977</v>
+      </c>
+      <c r="G3">
+        <v>0.6985583934814392</v>
+      </c>
+      <c r="H3">
+        <v>0.6817654642258674</v>
+      </c>
+      <c r="I3">
+        <v>0.5439349065121836</v>
+      </c>
+      <c r="J3">
+        <v>0.6118274768573116</v>
+      </c>
+      <c r="K3">
+        <v>0.6374758219755982</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0.8591591742252117</v>
+        <v>0.8425486947018774</v>
       </c>
       <c r="C4">
-        <v>0.7942991582195336</v>
+        <v>0.7864791828555581</v>
       </c>
       <c r="D4">
-        <v>0.7980607569483712</v>
+        <v>0.8052878858953885</v>
       </c>
       <c r="E4">
-        <v>0.8124340229702786</v>
+        <v>0.8661249249735148</v>
       </c>
       <c r="F4">
-        <v>0.8264914097711802</v>
+        <v>0.8413550144787181</v>
+      </c>
+      <c r="G4">
+        <v>0.7723485920790469</v>
+      </c>
+      <c r="H4">
+        <v>0.7580373529393835</v>
+      </c>
+      <c r="I4">
+        <v>0.8906154327761845</v>
+      </c>
+      <c r="J4">
+        <v>0.7716833961433427</v>
+      </c>
+      <c r="K4">
+        <v>0.7486562908830035</v>
       </c>
     </row>
   </sheetData>
@@ -473,13 +533,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:11">
       <c r="B1" s="1">
         <v>1</v>
       </c>
@@ -495,65 +555,125 @@
       <c r="F1" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" s="1">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>34.14199344112422</v>
+        <v>37.36937362360312</v>
       </c>
       <c r="C2">
-        <v>36.97797418323906</v>
+        <v>34.96575798684802</v>
       </c>
       <c r="D2">
-        <v>43.60367993483153</v>
+        <v>38.22814155549965</v>
       </c>
       <c r="E2">
-        <v>43.71941975396911</v>
+        <v>30.77963682037742</v>
       </c>
       <c r="F2">
-        <v>45.02993152570104</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>45.99958864690752</v>
+      </c>
+      <c r="G2">
+        <v>37.07694808593751</v>
+      </c>
+      <c r="H2">
+        <v>35.39087536173187</v>
+      </c>
+      <c r="I2">
+        <v>48.16734599379718</v>
+      </c>
+      <c r="J2">
+        <v>37.45436288791731</v>
+      </c>
+      <c r="K2">
+        <v>56.78045671557197</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.5736972780193429</v>
+        <v>0.7047525999704891</v>
       </c>
       <c r="C3">
-        <v>0.6760326787820042</v>
+        <v>0.649031809840943</v>
       </c>
       <c r="D3">
-        <v>0.6634873965022487</v>
+        <v>0.8487868204622602</v>
       </c>
       <c r="E3">
-        <v>0.6872904182538337</v>
+        <v>0.5887793081473495</v>
       </c>
       <c r="F3">
-        <v>0.6791143537792589</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>0.5812618797255628</v>
+      </c>
+      <c r="G3">
+        <v>0.6797799787069773</v>
+      </c>
+      <c r="H3">
+        <v>0.622816288230676</v>
+      </c>
+      <c r="I3">
+        <v>0.5739376998274894</v>
+      </c>
+      <c r="J3">
+        <v>0.6378962721133219</v>
+      </c>
+      <c r="K3">
+        <v>0.6561494821936028</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0.8226825358786287</v>
+        <v>0.7669945399419645</v>
       </c>
       <c r="C4">
-        <v>0.7362173928849625</v>
+        <v>0.8070986795002415</v>
       </c>
       <c r="D4">
-        <v>0.7922673212419951</v>
+        <v>0.7224971509741622</v>
       </c>
       <c r="E4">
-        <v>0.7891466293525875</v>
+        <v>0.8513704267667095</v>
       </c>
       <c r="F4">
-        <v>0.8178106763456218</v>
+        <v>0.830652097072924</v>
+      </c>
+      <c r="G4">
+        <v>0.7844233848021015</v>
+      </c>
+      <c r="H4">
+        <v>0.7980712040942353</v>
+      </c>
+      <c r="I4">
+        <v>0.8782155894845962</v>
+      </c>
+      <c r="J4">
+        <v>0.7518126339517133</v>
+      </c>
+      <c r="K4">
+        <v>0.7337153296528807</v>
       </c>
     </row>
   </sheetData>
@@ -563,13 +683,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:11">
       <c r="B1" s="1">
         <v>1</v>
       </c>
@@ -585,65 +705,125 @@
       <c r="F1" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" s="1">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>36.38925963521305</v>
+        <v>37.72818841984554</v>
       </c>
       <c r="C2">
-        <v>37.03215266106085</v>
+        <v>45.97664956604137</v>
       </c>
       <c r="D2">
-        <v>48.30128550544479</v>
+        <v>41.02222074193498</v>
       </c>
       <c r="E2">
-        <v>50.33066643996497</v>
+        <v>35.15516632073809</v>
       </c>
       <c r="F2">
-        <v>50.49461535703765</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>54.8614797959845</v>
+      </c>
+      <c r="G2">
+        <v>37.45214207266446</v>
+      </c>
+      <c r="H2">
+        <v>39.56353281943321</v>
+      </c>
+      <c r="I2">
+        <v>52.25110058982995</v>
+      </c>
+      <c r="J2">
+        <v>43.47459823000558</v>
+      </c>
+      <c r="K2">
+        <v>58.67119656657275</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.5611250454563</v>
+        <v>0.6937907726114121</v>
       </c>
       <c r="C3">
-        <v>0.6283018924344486</v>
+        <v>0.7378380885492311</v>
       </c>
       <c r="D3">
-        <v>0.711946874374134</v>
+        <v>0.8326363970159318</v>
       </c>
       <c r="E3">
-        <v>0.6843605401554367</v>
+        <v>0.6620307310516503</v>
       </c>
       <c r="F3">
-        <v>0.7606006420728547</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>0.6371260303711855</v>
+      </c>
+      <c r="G3">
+        <v>0.7288098208368927</v>
+      </c>
+      <c r="H3">
+        <v>0.6728500317966467</v>
+      </c>
+      <c r="I3">
+        <v>0.594097668205498</v>
+      </c>
+      <c r="J3">
+        <v>0.6417088637896213</v>
+      </c>
+      <c r="K3">
+        <v>0.6467913670257639</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0.8303689930111784</v>
+        <v>0.7741865721242489</v>
       </c>
       <c r="C4">
-        <v>0.7721507978000279</v>
+        <v>0.7506982216709186</v>
       </c>
       <c r="D4">
-        <v>0.7608146135954629</v>
+        <v>0.732957137976106</v>
       </c>
       <c r="E4">
-        <v>0.7909405082950313</v>
+        <v>0.8120871617810239</v>
       </c>
       <c r="F4">
-        <v>0.7714661798384864</v>
+        <v>0.7965363473213727</v>
+      </c>
+      <c r="G4">
+        <v>0.7522045415465047</v>
+      </c>
+      <c r="H4">
+        <v>0.7643242562892085</v>
+      </c>
+      <c r="I4">
+        <v>0.8695098025803693</v>
+      </c>
+      <c r="J4">
+        <v>0.7488370253075691</v>
+      </c>
+      <c r="K4">
+        <v>0.7412567590627132</v>
       </c>
     </row>
   </sheetData>
@@ -653,13 +833,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:11">
       <c r="B1" s="1">
         <v>1</v>
       </c>
@@ -675,65 +855,125 @@
       <c r="F1" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" s="1">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>54.02514426969353</v>
+        <v>49.49359112518707</v>
       </c>
       <c r="C2">
-        <v>59.66085686667097</v>
+        <v>61.96802891958342</v>
       </c>
       <c r="D2">
-        <v>59.78019895502647</v>
+        <v>55.56092945670751</v>
       </c>
       <c r="E2">
-        <v>68.21429838760751</v>
+        <v>54.86142324937349</v>
       </c>
       <c r="F2">
-        <v>72.52814927996546</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>71.22568683739945</v>
+      </c>
+      <c r="G2">
+        <v>47.83245738043706</v>
+      </c>
+      <c r="H2">
+        <v>54.03652176510341</v>
+      </c>
+      <c r="I2">
+        <v>90.69416180347929</v>
+      </c>
+      <c r="J2">
+        <v>61.89426987663489</v>
+      </c>
+      <c r="K2">
+        <v>72.23383286291525</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.7544589519627691</v>
+        <v>0.8143813899525644</v>
       </c>
       <c r="C3">
-        <v>0.815994613050641</v>
+        <v>0.8648189780504634</v>
       </c>
       <c r="D3">
-        <v>0.8314082654577082</v>
+        <v>0.8575473935589115</v>
       </c>
       <c r="E3">
-        <v>0.8024933012334423</v>
+        <v>0.8794596946131777</v>
       </c>
       <c r="F3">
-        <v>0.8727427256526339</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>0.750950727874952</v>
+      </c>
+      <c r="G3">
+        <v>0.8643342777671682</v>
+      </c>
+      <c r="H3">
+        <v>0.7963426989774348</v>
+      </c>
+      <c r="I3">
+        <v>0.8257256394722737</v>
+      </c>
+      <c r="J3">
+        <v>0.7254839807046519</v>
+      </c>
+      <c r="K3">
+        <v>0.8365870004528093</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0.6933399762283591</v>
+        <v>0.6888653311640482</v>
       </c>
       <c r="C4">
-        <v>0.6156867481500354</v>
+        <v>0.6575054554158579</v>
       </c>
       <c r="D4">
-        <v>0.6738118782939675</v>
+        <v>0.7167392153103405</v>
       </c>
       <c r="E4">
-        <v>0.7125364391094779</v>
+        <v>0.6683866283527444</v>
       </c>
       <c r="F4">
-        <v>0.69910873564985</v>
+        <v>0.7173434693014356</v>
+      </c>
+      <c r="G4">
+        <v>0.651479456005993</v>
+      </c>
+      <c r="H4">
+        <v>0.6698750585871875</v>
+      </c>
+      <c r="I4">
+        <v>0.7479227034049891</v>
+      </c>
+      <c r="J4">
+        <v>0.6789777041598343</v>
+      </c>
+      <c r="K4">
+        <v>0.5671246972442818</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed experimental models and got ensemble benchmarks
</commit_message>
<xml_diff>
--- a/Ensemble/ExperimentalModels/model_metrics.xlsx
+++ b/Ensemble/ExperimentalModels/model_metrics.xlsx
@@ -7,14 +7,17 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="gbr" sheetId="1" r:id="rId1"/>
+    <sheet name="svr" sheetId="1" r:id="rId1"/>
+    <sheet name="gbr" sheetId="2" r:id="rId2"/>
+    <sheet name="rf" sheetId="3" r:id="rId3"/>
+    <sheet name="lr" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="3">
   <si>
     <t>test_MAPE</t>
   </si>
@@ -423,34 +426,34 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>36.48055609448617</v>
+        <v>28.98029672317424</v>
       </c>
       <c r="C2">
-        <v>39.53173451468621</v>
+        <v>36.70850919668717</v>
       </c>
       <c r="D2">
-        <v>40.59305603432382</v>
+        <v>37.96986392644682</v>
       </c>
       <c r="E2">
-        <v>33.7565834032184</v>
+        <v>31.22592845419224</v>
       </c>
       <c r="F2">
-        <v>54.44234160264637</v>
+        <v>43.61157316185502</v>
       </c>
       <c r="G2">
-        <v>36.41771039324178</v>
+        <v>30.27784069838451</v>
       </c>
       <c r="H2">
-        <v>38.7279620379198</v>
+        <v>31.30217745473083</v>
       </c>
       <c r="I2">
-        <v>50.2452709599637</v>
+        <v>39.61213871867896</v>
       </c>
       <c r="J2">
-        <v>42.04442459251803</v>
+        <v>42.51503485461354</v>
       </c>
       <c r="K2">
-        <v>60.85422410531736</v>
+        <v>54.25680821473518</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -458,34 +461,34 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.7051181415267634</v>
+        <v>0.5793310029159989</v>
       </c>
       <c r="C3">
-        <v>0.6683176370305869</v>
+        <v>0.6828392768481389</v>
       </c>
       <c r="D3">
-        <v>0.8011288749327667</v>
+        <v>0.7109865587139155</v>
       </c>
       <c r="E3">
-        <v>0.6195709184260487</v>
+        <v>0.5587914946739748</v>
       </c>
       <c r="F3">
-        <v>0.6263455677578484</v>
+        <v>0.5625940117129977</v>
       </c>
       <c r="G3">
-        <v>0.7123841937937564</v>
+        <v>0.6985583934814392</v>
       </c>
       <c r="H3">
-        <v>0.6429295653988311</v>
+        <v>0.6817654642258674</v>
       </c>
       <c r="I3">
-        <v>0.5475779053334122</v>
+        <v>0.5439349065121836</v>
       </c>
       <c r="J3">
-        <v>0.6789309869817534</v>
+        <v>0.6118274768573116</v>
       </c>
       <c r="K3">
-        <v>0.7041347213146948</v>
+        <v>0.6374758219755982</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -493,34 +496,484 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0.7667527663966536</v>
+        <v>0.8425486947018774</v>
       </c>
       <c r="C4">
-        <v>0.7954643194529789</v>
+        <v>0.7864791828555581</v>
       </c>
       <c r="D4">
-        <v>0.7527849184058867</v>
+        <v>0.8052878858953885</v>
       </c>
       <c r="E4">
-        <v>0.8354180505934956</v>
+        <v>0.8661249249735148</v>
       </c>
       <c r="F4">
-        <v>0.8033634906507463</v>
+        <v>0.8413550144787181</v>
       </c>
       <c r="G4">
-        <v>0.7632481072020412</v>
+        <v>0.7723485920790469</v>
       </c>
       <c r="H4">
-        <v>0.784818402890391</v>
+        <v>0.7580373529393835</v>
       </c>
       <c r="I4">
-        <v>0.88914532200026</v>
+        <v>0.8906154327761845</v>
       </c>
       <c r="J4">
-        <v>0.7188547158719667</v>
+        <v>0.7716833961433427</v>
       </c>
       <c r="K4">
-        <v>0.693343549217876</v>
+        <v>0.7486562908830035</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:K4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="B1" s="1">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>36.66940396061146</v>
+      </c>
+      <c r="C2">
+        <v>39.74081284661591</v>
+      </c>
+      <c r="D2">
+        <v>40.51819336104671</v>
+      </c>
+      <c r="E2">
+        <v>33.4588648628547</v>
+      </c>
+      <c r="F2">
+        <v>54.93869916141576</v>
+      </c>
+      <c r="G2">
+        <v>36.90295354976845</v>
+      </c>
+      <c r="H2">
+        <v>38.30998902630365</v>
+      </c>
+      <c r="I2">
+        <v>49.70818358900601</v>
+      </c>
+      <c r="J2">
+        <v>42.03943076969593</v>
+      </c>
+      <c r="K2">
+        <v>58.57689376388119</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>0.7059232209729004</v>
+      </c>
+      <c r="C3">
+        <v>0.6743553102633484</v>
+      </c>
+      <c r="D3">
+        <v>0.7990510377788524</v>
+      </c>
+      <c r="E3">
+        <v>0.6081931944553557</v>
+      </c>
+      <c r="F3">
+        <v>0.6334673370109501</v>
+      </c>
+      <c r="G3">
+        <v>0.7105551418038231</v>
+      </c>
+      <c r="H3">
+        <v>0.6395539074198077</v>
+      </c>
+      <c r="I3">
+        <v>0.5343578120736606</v>
+      </c>
+      <c r="J3">
+        <v>0.6779399706971465</v>
+      </c>
+      <c r="K3">
+        <v>0.6846128162732461</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>0.7662198351206548</v>
+      </c>
+      <c r="C4">
+        <v>0.7917520193387215</v>
+      </c>
+      <c r="D4">
+        <v>0.7540656275588534</v>
+      </c>
+      <c r="E4">
+        <v>0.8414072735600724</v>
+      </c>
+      <c r="F4">
+        <v>0.7988664160706718</v>
+      </c>
+      <c r="G4">
+        <v>0.7644622711840667</v>
+      </c>
+      <c r="H4">
+        <v>0.7870720636681269</v>
+      </c>
+      <c r="I4">
+        <v>0.8944334038620378</v>
+      </c>
+      <c r="J4">
+        <v>0.7196748764294405</v>
+      </c>
+      <c r="K4">
+        <v>0.7101117352046091</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:K4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="B1" s="1">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>37.42320813651045</v>
+      </c>
+      <c r="C2">
+        <v>45.52441340309524</v>
+      </c>
+      <c r="D2">
+        <v>41.20858145545606</v>
+      </c>
+      <c r="E2">
+        <v>35.25538993554812</v>
+      </c>
+      <c r="F2">
+        <v>54.45113021035772</v>
+      </c>
+      <c r="G2">
+        <v>37.42371588731501</v>
+      </c>
+      <c r="H2">
+        <v>39.43524670297821</v>
+      </c>
+      <c r="I2">
+        <v>52.91098182335776</v>
+      </c>
+      <c r="J2">
+        <v>43.23115316427026</v>
+      </c>
+      <c r="K2">
+        <v>59.51435247832557</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>0.6987807504861013</v>
+      </c>
+      <c r="C3">
+        <v>0.733546665028436</v>
+      </c>
+      <c r="D3">
+        <v>0.8342113916219497</v>
+      </c>
+      <c r="E3">
+        <v>0.6749140963990878</v>
+      </c>
+      <c r="F3">
+        <v>0.6434318612900801</v>
+      </c>
+      <c r="G3">
+        <v>0.7292890445889028</v>
+      </c>
+      <c r="H3">
+        <v>0.6754216659060778</v>
+      </c>
+      <c r="I3">
+        <v>0.5900103775610548</v>
+      </c>
+      <c r="J3">
+        <v>0.6375841783150619</v>
+      </c>
+      <c r="K3">
+        <v>0.6526142609568413</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>0.7709266377713944</v>
+      </c>
+      <c r="C4">
+        <v>0.753589772720978</v>
+      </c>
+      <c r="D4">
+        <v>0.7319459190127015</v>
+      </c>
+      <c r="E4">
+        <v>0.8047022899711458</v>
+      </c>
+      <c r="F4">
+        <v>0.7924889328743652</v>
+      </c>
+      <c r="G4">
+        <v>0.7518785621006396</v>
+      </c>
+      <c r="H4">
+        <v>0.7625193073218292</v>
+      </c>
+      <c r="I4">
+        <v>0.8712991268222839</v>
+      </c>
+      <c r="J4">
+        <v>0.7520554282518258</v>
+      </c>
+      <c r="K4">
+        <v>0.7365769923158358</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:K4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="B1" s="1">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>49.49359112518707</v>
+      </c>
+      <c r="C2">
+        <v>61.96802891958342</v>
+      </c>
+      <c r="D2">
+        <v>55.56092945670751</v>
+      </c>
+      <c r="E2">
+        <v>54.86142324937349</v>
+      </c>
+      <c r="F2">
+        <v>71.22568683739945</v>
+      </c>
+      <c r="G2">
+        <v>47.83245738043706</v>
+      </c>
+      <c r="H2">
+        <v>54.03652176510341</v>
+      </c>
+      <c r="I2">
+        <v>90.69416180347929</v>
+      </c>
+      <c r="J2">
+        <v>61.89426987663489</v>
+      </c>
+      <c r="K2">
+        <v>72.23383286291525</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>0.8143813899525644</v>
+      </c>
+      <c r="C3">
+        <v>0.8648189780504634</v>
+      </c>
+      <c r="D3">
+        <v>0.8575473935589115</v>
+      </c>
+      <c r="E3">
+        <v>0.8794596946131777</v>
+      </c>
+      <c r="F3">
+        <v>0.750950727874952</v>
+      </c>
+      <c r="G3">
+        <v>0.8643342777671682</v>
+      </c>
+      <c r="H3">
+        <v>0.7963426989774348</v>
+      </c>
+      <c r="I3">
+        <v>0.8257256394722737</v>
+      </c>
+      <c r="J3">
+        <v>0.7254839807046519</v>
+      </c>
+      <c r="K3">
+        <v>0.8365870004528093</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>0.6888653311640482</v>
+      </c>
+      <c r="C4">
+        <v>0.6575054554158579</v>
+      </c>
+      <c r="D4">
+        <v>0.7167392153103405</v>
+      </c>
+      <c r="E4">
+        <v>0.6683866283527444</v>
+      </c>
+      <c r="F4">
+        <v>0.7173434693014356</v>
+      </c>
+      <c r="G4">
+        <v>0.651479456005993</v>
+      </c>
+      <c r="H4">
+        <v>0.6698750585871875</v>
+      </c>
+      <c r="I4">
+        <v>0.7479227034049891</v>
+      </c>
+      <c r="J4">
+        <v>0.6789777041598343</v>
+      </c>
+      <c r="K4">
+        <v>0.5671246972442818</v>
       </c>
     </row>
   </sheetData>

</xml_diff>